<commit_message>
Couple new AI types and updated timelog
</commit_message>
<xml_diff>
--- a/SD4_kkleber_sohlrich_rsanders_sspangler/SD4_kkleber_sohlrich_rsanders_sspangler/Documents/SD4_SSpangler_Timelog.xlsx
+++ b/SD4_kkleber_sohlrich_rsanders_sspangler/SD4_kkleber_sohlrich_rsanders_sspangler/Documents/SD4_SSpangler_Timelog.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Project Time Log:</t>
   </si>
@@ -151,6 +151,15 @@
   </si>
   <si>
     <t>Code</t>
+  </si>
+  <si>
+    <t>Testing above scripts</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Fleeing, Shooting, berserk</t>
   </si>
 </sst>
 </file>
@@ -685,7 +694,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -697,7 +706,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -740,7 +749,7 @@
       <c r="C3" s="10"/>
       <c r="H3" s="12">
         <f>SUM(G12:G120)</f>
-        <v>5.0694444444444597E-2</v>
+        <v>7.0138888888888973E-2</v>
       </c>
       <c r="I3" t="s">
         <v>3</v>
@@ -753,7 +762,7 @@
       <c r="C4" s="14"/>
       <c r="H4" s="15">
         <f>(INT(H3*24))+MINUTE(H3)/60</f>
-        <v>1.2166666666666668</v>
+        <v>1.6833333333333333</v>
       </c>
       <c r="I4" t="s">
         <v>3</v>
@@ -879,11 +888,32 @@
         <f t="shared" ref="G13:G76" si="0">(E13-D13)-(F13/1440)</f>
         <v>6.9444444444445308E-3</v>
       </c>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="14" spans="1:10">
+      <c r="C14" s="3">
+        <v>42114</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.9159722222222223</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0.93541666666666667</v>
+      </c>
       <c r="G14" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.9444444444444375E-2</v>
+      </c>
+      <c r="H14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:10">

</xml_diff>

<commit_message>
Added solo mode and added up level up functionality
</commit_message>
<xml_diff>
--- a/SD4_kkleber_sohlrich_rsanders_sspangler/SD4_kkleber_sohlrich_rsanders_sspangler/Documents/SD4_SSpangler_Timelog.xlsx
+++ b/SD4_kkleber_sohlrich_rsanders_sspangler/SD4_kkleber_sohlrich_rsanders_sspangler/Documents/SD4_SSpangler_Timelog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="9030"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23460" windowHeight="8625"/>
   </bookViews>
   <sheets>
     <sheet name="Time Log" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Project Time Log:</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>Tested bosses</t>
+  </si>
+  <si>
+    <t>Coding for collisions with enemies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing to make sure code works </t>
   </si>
 </sst>
 </file>
@@ -703,7 +709,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -715,7 +721,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -758,7 +764,7 @@
       <c r="C3" s="10"/>
       <c r="H3" s="12">
         <f>SUM(G12:G120)</f>
-        <v>0.21666666666666667</v>
+        <v>0.2583333333333333</v>
       </c>
       <c r="I3" t="s">
         <v>3</v>
@@ -771,7 +777,7 @@
       <c r="C4" s="14"/>
       <c r="H4" s="15">
         <f>(INT(H3*24))+MINUTE(H3)/60</f>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="I4" t="s">
         <v>3</v>
@@ -1010,15 +1016,45 @@
       </c>
     </row>
     <row r="19" spans="3:9">
+      <c r="C19" s="3">
+        <v>42123</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="G19" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.125E-2</v>
+      </c>
+      <c r="H19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="3:9">
+      <c r="C20" s="3">
+        <v>42123</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0.71875</v>
+      </c>
       <c r="G20" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="H20" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="3:9">

</xml_diff>